<commit_message>
[Upd] Updated rules, etc
</commit_message>
<xml_diff>
--- a/output/test-edges.xlsx
+++ b/output/test-edges.xlsx
@@ -771,7 +771,7 @@
         <v>11</v>
       </c>
       <c r="E3">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -822,7 +822,7 @@
         <v>21</v>
       </c>
       <c r="E6">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -839,7 +839,7 @@
         <v>15</v>
       </c>
       <c r="E7">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -890,7 +890,7 @@
         <v>15</v>
       </c>
       <c r="E10">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -907,7 +907,7 @@
         <v>15</v>
       </c>
       <c r="E11">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -941,7 +941,7 @@
         <v>15</v>
       </c>
       <c r="E13">
-        <v>38.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -958,7 +958,7 @@
         <v>43</v>
       </c>
       <c r="E14">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -992,7 +992,7 @@
         <v>49</v>
       </c>
       <c r="E16">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1009,7 +1009,7 @@
         <v>15</v>
       </c>
       <c r="E17">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1026,7 +1026,7 @@
         <v>53</v>
       </c>
       <c r="E18">
-        <v>3.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1111,7 +1111,7 @@
         <v>15</v>
       </c>
       <c r="E23">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1128,7 +1128,7 @@
         <v>11</v>
       </c>
       <c r="E24">
-        <v>2.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1145,7 +1145,7 @@
         <v>73</v>
       </c>
       <c r="E25">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -1162,7 +1162,7 @@
         <v>76</v>
       </c>
       <c r="E26">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -1179,7 +1179,7 @@
         <v>78</v>
       </c>
       <c r="E27">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -1196,7 +1196,7 @@
         <v>15</v>
       </c>
       <c r="E28">
-        <v>2.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -1213,7 +1213,7 @@
         <v>83</v>
       </c>
       <c r="E29">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -1281,7 +1281,7 @@
         <v>15</v>
       </c>
       <c r="E33">
-        <v>21</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -1298,7 +1298,7 @@
         <v>11</v>
       </c>
       <c r="E34">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -1315,7 +1315,7 @@
         <v>11</v>
       </c>
       <c r="E35">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -1332,7 +1332,7 @@
         <v>99</v>
       </c>
       <c r="E36">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1349,7 +1349,7 @@
         <v>11</v>
       </c>
       <c r="E37">
-        <v>4.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1366,7 +1366,7 @@
         <v>15</v>
       </c>
       <c r="E38">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -1400,7 +1400,7 @@
         <v>109</v>
       </c>
       <c r="E40">
-        <v>5.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1417,7 +1417,7 @@
         <v>99</v>
       </c>
       <c r="E41">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -1468,7 +1468,7 @@
         <v>15</v>
       </c>
       <c r="E44">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:5">

</xml_diff>

<commit_message>
[New] Abstracted groups picking from the context
</commit_message>
<xml_diff>
--- a/output/test-edges.xlsx
+++ b/output/test-edges.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="83">
   <si>
     <t>Source</t>
   </si>
@@ -88,90 +88,39 @@
     <t>part-&gt;drive</t>
   </si>
   <si>
+    <t>island</t>
+  </si>
+  <si>
+    <t>island-&gt;democracy</t>
+  </si>
+  <si>
+    <t>law</t>
+  </si>
+  <si>
+    <t>use</t>
+  </si>
+  <si>
+    <t>law-&gt;use</t>
+  </si>
+  <si>
+    <t>requiring</t>
+  </si>
+  <si>
+    <t>use-&gt;ink</t>
+  </si>
+  <si>
+    <t>parliamentary</t>
+  </si>
+  <si>
+    <t>ink-&gt;parliamentary</t>
+  </si>
+  <si>
+    <t>during</t>
+  </si>
+  <si>
     <t>technology</t>
   </si>
   <si>
-    <t>worries</t>
-  </si>
-  <si>
-    <t>technology-&gt;worries</t>
-  </si>
-  <si>
-    <t>is causing</t>
-  </si>
-  <si>
-    <t>optimism</t>
-  </si>
-  <si>
-    <t>sectors</t>
-  </si>
-  <si>
-    <t>optimism-&gt;sectors</t>
-  </si>
-  <si>
-    <t>among</t>
-  </si>
-  <si>
-    <t>population</t>
-  </si>
-  <si>
-    <t>sectors-&gt;population</t>
-  </si>
-  <si>
-    <t>island</t>
-  </si>
-  <si>
-    <t>island-&gt;democracy</t>
-  </si>
-  <si>
-    <t>law</t>
-  </si>
-  <si>
-    <t>use</t>
-  </si>
-  <si>
-    <t>law-&gt;use</t>
-  </si>
-  <si>
-    <t>requiring</t>
-  </si>
-  <si>
-    <t>use-&gt;ink</t>
-  </si>
-  <si>
-    <t>parliamentary</t>
-  </si>
-  <si>
-    <t>ink-&gt;parliamentary</t>
-  </si>
-  <si>
-    <t>during</t>
-  </si>
-  <si>
-    <t>experts</t>
-  </si>
-  <si>
-    <t>backsliding</t>
-  </si>
-  <si>
-    <t>experts-&gt;backsliding</t>
-  </si>
-  <si>
-    <t>point</t>
-  </si>
-  <si>
-    <t>backsliding-&gt;point</t>
-  </si>
-  <si>
-    <t>from</t>
-  </si>
-  <si>
-    <t>effort</t>
-  </si>
-  <si>
-    <t>part-&gt;effort</t>
-  </si>
-  <si>
     <t>technology-&gt;ink</t>
   </si>
   <si>
@@ -253,12 +202,6 @@
     <t>against</t>
   </si>
   <si>
-    <t>opposition</t>
-  </si>
-  <si>
-    <t>part-&gt;opposition</t>
-  </si>
-  <si>
     <t>stories</t>
   </si>
   <si>
@@ -268,33 +211,6 @@
     <t>that</t>
   </si>
   <si>
-    <t>middle</t>
-  </si>
-  <si>
-    <t>road</t>
-  </si>
-  <si>
-    <t>middle-&gt;road</t>
-  </si>
-  <si>
-    <t>coalition</t>
-  </si>
-  <si>
-    <t>organizations</t>
-  </si>
-  <si>
-    <t>coalition-&gt;organizations</t>
-  </si>
-  <si>
-    <t>move</t>
-  </si>
-  <si>
-    <t>step</t>
-  </si>
-  <si>
-    <t>move-&gt;step</t>
-  </si>
-  <si>
     <t>type</t>
   </si>
   <si>
@@ -325,18 +241,6 @@
     <t>use-&gt;type</t>
   </si>
   <si>
-    <t>leaders</t>
-  </si>
-  <si>
-    <t>populations</t>
-  </si>
-  <si>
-    <t>leaders-&gt;populations</t>
-  </si>
-  <si>
-    <t>assured their</t>
-  </si>
-  <si>
     <t>contrary</t>
   </si>
   <si>
@@ -359,33 +263,6 @@
   </si>
   <si>
     <t>cuticle-&gt;thumb</t>
-  </si>
-  <si>
-    <t>panacea</t>
-  </si>
-  <si>
-    <t>ills</t>
-  </si>
-  <si>
-    <t>panacea-&gt;ills</t>
-  </si>
-  <si>
-    <t>for</t>
-  </si>
-  <si>
-    <t>passage</t>
-  </si>
-  <si>
-    <t>passage-&gt;law</t>
-  </si>
-  <si>
-    <t>building</t>
-  </si>
-  <si>
-    <t>societies</t>
-  </si>
-  <si>
-    <t>building-&gt;societies</t>
   </si>
 </sst>
 </file>
@@ -717,7 +594,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -847,13 +724,13 @@
         <v>24</v>
       </c>
       <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
         <v>25</v>
       </c>
-      <c r="C8" t="s">
-        <v>26</v>
-      </c>
       <c r="D8" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -861,16 +738,16 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" t="s">
         <v>28</v>
       </c>
-      <c r="B9" t="s">
+      <c r="D9" t="s">
         <v>29</v>
-      </c>
-      <c r="C9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" t="s">
-        <v>31</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -878,13 +755,13 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D10" t="s">
         <v>15</v>
@@ -895,16 +772,16 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -912,16 +789,16 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" t="s">
         <v>36</v>
-      </c>
-      <c r="B12" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" t="s">
-        <v>39</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -932,10 +809,10 @@
         <v>37</v>
       </c>
       <c r="B13" t="s">
-        <v>5</v>
+        <v>38</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D13" t="s">
         <v>15</v>
@@ -946,7 +823,7 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="B14" t="s">
         <v>41</v>
@@ -972,7 +849,7 @@
         <v>46</v>
       </c>
       <c r="D15" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -980,16 +857,16 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B16" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C16" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D16" t="s">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -997,10 +874,10 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="B17" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
       <c r="C17" t="s">
         <v>51</v>
@@ -1014,16 +891,16 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>5</v>
+        <v>52</v>
       </c>
       <c r="C18" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D18" t="s">
-        <v>53</v>
+        <v>11</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -1034,13 +911,13 @@
         <v>54</v>
       </c>
       <c r="B19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" t="s">
         <v>55</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>56</v>
-      </c>
-      <c r="D19" t="s">
-        <v>15</v>
       </c>
       <c r="E19">
         <v>1</v>
@@ -1051,13 +928,13 @@
         <v>57</v>
       </c>
       <c r="B20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" t="s">
         <v>58</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>59</v>
-      </c>
-      <c r="D20" t="s">
-        <v>60</v>
       </c>
       <c r="E20">
         <v>1</v>
@@ -1065,16 +942,16 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D21" t="s">
         <v>61</v>
-      </c>
-      <c r="B21" t="s">
-        <v>62</v>
-      </c>
-      <c r="C21" t="s">
-        <v>63</v>
-      </c>
-      <c r="D21" t="s">
-        <v>55</v>
       </c>
       <c r="E21">
         <v>1</v>
@@ -1082,16 +959,16 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" t="s">
+        <v>63</v>
+      </c>
+      <c r="D22" t="s">
         <v>64</v>
-      </c>
-      <c r="B22" t="s">
-        <v>65</v>
-      </c>
-      <c r="C22" t="s">
-        <v>66</v>
-      </c>
-      <c r="D22" t="s">
-        <v>11</v>
       </c>
       <c r="E22">
         <v>1</v>
@@ -1099,13 +976,13 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B23" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="C23" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D23" t="s">
         <v>15</v>
@@ -1119,10 +996,10 @@
         <v>17</v>
       </c>
       <c r="B24" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C24" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D24" t="s">
         <v>11</v>
@@ -1133,16 +1010,16 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>71</v>
+        <v>5</v>
       </c>
       <c r="B25" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="C25" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D25" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="E25">
         <v>1</v>
@@ -1150,16 +1027,16 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>74</v>
+        <v>17</v>
       </c>
       <c r="B26" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="C26" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D26" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E26">
         <v>1</v>
@@ -1167,16 +1044,16 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B27" t="s">
-        <v>37</v>
+        <v>72</v>
       </c>
       <c r="C27" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D27" t="s">
-        <v>78</v>
+        <v>11</v>
       </c>
       <c r="E27">
         <v>1</v>
@@ -1184,13 +1061,13 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="C28" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D28" t="s">
         <v>15</v>
@@ -1201,16 +1078,16 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>81</v>
+        <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>5</v>
+        <v>75</v>
       </c>
       <c r="C29" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D29" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="E29">
         <v>1</v>
@@ -1218,16 +1095,16 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>84</v>
+        <v>5</v>
       </c>
       <c r="B30" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C30" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="D30" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
       <c r="E30">
         <v>1</v>
@@ -1235,256 +1112,18 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="B31" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C31" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D31" t="s">
         <v>15</v>
       </c>
       <c r="E31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" t="s">
-        <v>90</v>
-      </c>
-      <c r="B32" t="s">
-        <v>91</v>
-      </c>
-      <c r="C32" t="s">
-        <v>92</v>
-      </c>
-      <c r="D32" t="s">
-        <v>21</v>
-      </c>
-      <c r="E32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33" t="s">
-        <v>93</v>
-      </c>
-      <c r="B33" t="s">
-        <v>5</v>
-      </c>
-      <c r="C33" t="s">
-        <v>94</v>
-      </c>
-      <c r="D33" t="s">
-        <v>15</v>
-      </c>
-      <c r="E33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" t="s">
-        <v>17</v>
-      </c>
-      <c r="B34" t="s">
-        <v>95</v>
-      </c>
-      <c r="C34" t="s">
-        <v>96</v>
-      </c>
-      <c r="D34" t="s">
-        <v>11</v>
-      </c>
-      <c r="E34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35" t="s">
-        <v>5</v>
-      </c>
-      <c r="B35" t="s">
-        <v>17</v>
-      </c>
-      <c r="C35" t="s">
-        <v>97</v>
-      </c>
-      <c r="D35" t="s">
-        <v>11</v>
-      </c>
-      <c r="E35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36" t="s">
-        <v>17</v>
-      </c>
-      <c r="B36" t="s">
-        <v>5</v>
-      </c>
-      <c r="C36" t="s">
-        <v>98</v>
-      </c>
-      <c r="D36" t="s">
-        <v>99</v>
-      </c>
-      <c r="E36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="A37" t="s">
-        <v>17</v>
-      </c>
-      <c r="B37" t="s">
-        <v>100</v>
-      </c>
-      <c r="C37" t="s">
-        <v>101</v>
-      </c>
-      <c r="D37" t="s">
-        <v>11</v>
-      </c>
-      <c r="E37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="A38" t="s">
-        <v>37</v>
-      </c>
-      <c r="B38" t="s">
-        <v>93</v>
-      </c>
-      <c r="C38" t="s">
-        <v>102</v>
-      </c>
-      <c r="D38" t="s">
-        <v>15</v>
-      </c>
-      <c r="E38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
-      <c r="A39" t="s">
-        <v>103</v>
-      </c>
-      <c r="B39" t="s">
-        <v>104</v>
-      </c>
-      <c r="C39" t="s">
-        <v>105</v>
-      </c>
-      <c r="D39" t="s">
-        <v>106</v>
-      </c>
-      <c r="E39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
-      <c r="A40" t="s">
-        <v>37</v>
-      </c>
-      <c r="B40" t="s">
-        <v>107</v>
-      </c>
-      <c r="C40" t="s">
-        <v>108</v>
-      </c>
-      <c r="D40" t="s">
-        <v>109</v>
-      </c>
-      <c r="E40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
-      <c r="A41" t="s">
-        <v>5</v>
-      </c>
-      <c r="B41" t="s">
-        <v>110</v>
-      </c>
-      <c r="C41" t="s">
-        <v>111</v>
-      </c>
-      <c r="D41" t="s">
-        <v>99</v>
-      </c>
-      <c r="E41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5">
-      <c r="A42" t="s">
-        <v>112</v>
-      </c>
-      <c r="B42" t="s">
-        <v>113</v>
-      </c>
-      <c r="C42" t="s">
-        <v>114</v>
-      </c>
-      <c r="D42" t="s">
-        <v>15</v>
-      </c>
-      <c r="E42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
-      <c r="A43" t="s">
-        <v>115</v>
-      </c>
-      <c r="B43" t="s">
-        <v>116</v>
-      </c>
-      <c r="C43" t="s">
-        <v>117</v>
-      </c>
-      <c r="D43" t="s">
-        <v>118</v>
-      </c>
-      <c r="E43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5">
-      <c r="A44" t="s">
-        <v>119</v>
-      </c>
-      <c r="B44" t="s">
-        <v>36</v>
-      </c>
-      <c r="C44" t="s">
-        <v>120</v>
-      </c>
-      <c r="D44" t="s">
-        <v>15</v>
-      </c>
-      <c r="E44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5">
-      <c r="A45" t="s">
-        <v>121</v>
-      </c>
-      <c r="B45" t="s">
-        <v>122</v>
-      </c>
-      <c r="C45" t="s">
-        <v>123</v>
-      </c>
-      <c r="D45" t="s">
-        <v>15</v>
-      </c>
-      <c r="E45">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[New] A couple of new rules
</commit_message>
<xml_diff>
--- a/output/test-edges.xlsx
+++ b/output/test-edges.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="94">
   <si>
     <t>Source</t>
   </si>
@@ -151,12 +151,36 @@
     <t>uv</t>
   </si>
   <si>
+    <t>ink-&gt;uv</t>
+  </si>
+  <si>
+    <t>shows under</t>
+  </si>
+  <si>
     <t>voter</t>
   </si>
   <si>
     <t>uv-&gt;voter</t>
   </si>
   <si>
+    <t>significance</t>
+  </si>
+  <si>
+    <t>elections-&gt;significance</t>
+  </si>
+  <si>
+    <t>are assuming</t>
+  </si>
+  <si>
+    <t>prelude</t>
+  </si>
+  <si>
+    <t>elections-&gt;prelude</t>
+  </si>
+  <si>
+    <t>are</t>
+  </si>
+  <si>
     <t>election</t>
   </si>
   <si>
@@ -263,6 +287,15 @@
   </si>
   <si>
     <t>cuticle-&gt;thumb</t>
+  </si>
+  <si>
+    <t>finger</t>
+  </si>
+  <si>
+    <t>ink-&gt;finger</t>
+  </si>
+  <si>
+    <t>stays on</t>
   </si>
 </sst>
 </file>
@@ -594,7 +627,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -840,16 +873,16 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
         <v>44</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>45</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>46</v>
-      </c>
-      <c r="D15" t="s">
-        <v>38</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -857,16 +890,16 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" t="s">
         <v>47</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>48</v>
       </c>
-      <c r="C16" t="s">
-        <v>49</v>
-      </c>
       <c r="D16" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -874,16 +907,16 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" t="s">
         <v>50</v>
       </c>
-      <c r="B17" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>51</v>
-      </c>
-      <c r="D17" t="s">
-        <v>15</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -900,7 +933,7 @@
         <v>53</v>
       </c>
       <c r="D18" t="s">
-        <v>11</v>
+        <v>54</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -908,16 +941,16 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B19" t="s">
-        <v>27</v>
+        <v>56</v>
       </c>
       <c r="C19" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D19" t="s">
-        <v>56</v>
+        <v>11</v>
       </c>
       <c r="E19">
         <v>1</v>
@@ -925,16 +958,16 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B20" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C20" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D20" t="s">
-        <v>59</v>
+        <v>15</v>
       </c>
       <c r="E20">
         <v>1</v>
@@ -942,16 +975,16 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B21" t="s">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="C21" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D21" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
       <c r="E21">
         <v>1</v>
@@ -962,7 +995,7 @@
         <v>62</v>
       </c>
       <c r="B22" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="C22" t="s">
         <v>63</v>
@@ -979,13 +1012,13 @@
         <v>65</v>
       </c>
       <c r="B23" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C23" t="s">
         <v>66</v>
       </c>
       <c r="D23" t="s">
-        <v>15</v>
+        <v>67</v>
       </c>
       <c r="E23">
         <v>1</v>
@@ -993,16 +1026,16 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>67</v>
+        <v>27</v>
       </c>
       <c r="C24" t="s">
         <v>68</v>
       </c>
       <c r="D24" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="E24">
         <v>1</v>
@@ -1010,16 +1043,16 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
+        <v>70</v>
+      </c>
+      <c r="B25" t="s">
         <v>5</v>
       </c>
-      <c r="B25" t="s">
-        <v>17</v>
-      </c>
       <c r="C25" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D25" t="s">
-        <v>11</v>
+        <v>72</v>
       </c>
       <c r="E25">
         <v>1</v>
@@ -1027,16 +1060,16 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>17</v>
+        <v>73</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>
       </c>
       <c r="C26" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="D26" t="s">
-        <v>71</v>
+        <v>15</v>
       </c>
       <c r="E26">
         <v>1</v>
@@ -1047,10 +1080,10 @@
         <v>17</v>
       </c>
       <c r="B27" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C27" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="D27" t="s">
         <v>11</v>
@@ -1061,16 +1094,16 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="B28" t="s">
-        <v>65</v>
+        <v>17</v>
       </c>
       <c r="C28" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="D28" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E28">
         <v>1</v>
@@ -1078,16 +1111,16 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="B29" t="s">
-        <v>75</v>
+        <v>5</v>
       </c>
       <c r="C29" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D29" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E29">
         <v>1</v>
@@ -1095,16 +1128,16 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B30" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C30" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D30" t="s">
-        <v>71</v>
+        <v>11</v>
       </c>
       <c r="E30">
         <v>1</v>
@@ -1112,10 +1145,10 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="s">
-        <v>80</v>
+        <v>27</v>
       </c>
       <c r="B31" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C31" t="s">
         <v>82</v>
@@ -1124,6 +1157,74 @@
         <v>15</v>
       </c>
       <c r="E31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" t="s">
+        <v>27</v>
+      </c>
+      <c r="B32" t="s">
+        <v>83</v>
+      </c>
+      <c r="C32" t="s">
+        <v>84</v>
+      </c>
+      <c r="D32" t="s">
+        <v>85</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" t="s">
+        <v>86</v>
+      </c>
+      <c r="C33" t="s">
+        <v>87</v>
+      </c>
+      <c r="D33" t="s">
+        <v>79</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" t="s">
+        <v>88</v>
+      </c>
+      <c r="B34" t="s">
+        <v>89</v>
+      </c>
+      <c r="C34" t="s">
+        <v>90</v>
+      </c>
+      <c r="D34" t="s">
+        <v>15</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35" t="s">
+        <v>91</v>
+      </c>
+      <c r="C35" t="s">
+        <v>92</v>
+      </c>
+      <c r="D35" t="s">
+        <v>93</v>
+      </c>
+      <c r="E35">
         <v>1</v>
       </c>
     </row>

</xml_diff>